<commit_message>
Zeitabschaetzung und timetable editiert
</commit_message>
<xml_diff>
--- a/Dokumente/Arbeitszeiterfassung1.xlsx
+++ b/Dokumente/Arbeitszeiterfassung1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Klune\Documents\5. Klasse\APR\Aufgaben\Aufgabe 8\Repo\RMIAuction\Dokumente\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22185" windowHeight="15480" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22188" windowHeight="15480" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Schuschnig" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
     <sheet name="Poelzlbauer" sheetId="5" r:id="rId5"/>
     <sheet name="Rieppel" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="152511" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
   <si>
     <t>Tobias Schuschnig</t>
   </si>
@@ -99,6 +104,12 @@
   </si>
   <si>
     <t>Erste Testfälle</t>
+  </si>
+  <si>
+    <t>27. Januar 2014</t>
+  </si>
+  <si>
+    <t>Use Case</t>
   </si>
 </sst>
 </file>
@@ -320,6 +331,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -647,7 +661,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K32"/>
@@ -656,16 +670,16 @@
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="42.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -680,7 +694,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -693,7 +707,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
@@ -702,7 +716,7 @@
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -719,7 +733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>41661</v>
       </c>
@@ -737,7 +751,7 @@
         <v>0.10416666666666696</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>41664</v>
       </c>
@@ -755,7 +769,7 @@
         <v>0.15972222222222199</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>41665</v>
       </c>
@@ -773,7 +787,7 @@
         <v>4.1666666666666075E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>41666</v>
       </c>
@@ -791,7 +805,7 @@
         <v>9.722222222222221E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
@@ -801,7 +815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="8"/>
       <c r="C10" s="7"/>
@@ -811,7 +825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="8"/>
       <c r="C11" s="7"/>
@@ -821,7 +835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="8"/>
       <c r="C12" s="7"/>
@@ -831,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="8"/>
       <c r="C13" s="7"/>
@@ -841,7 +855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="8"/>
       <c r="C14" s="7"/>
@@ -851,7 +865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="8"/>
       <c r="C15" s="7"/>
@@ -861,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="8"/>
       <c r="C16" s="7"/>
@@ -871,7 +885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="8"/>
       <c r="C17" s="7"/>
@@ -881,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="8"/>
       <c r="C18" s="7"/>
@@ -891,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="8"/>
       <c r="C19" s="7"/>
@@ -901,7 +915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="8"/>
       <c r="C20" s="7"/>
@@ -911,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -921,7 +935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -931,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -941,7 +955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -951,7 +965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -961,7 +975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -971,7 +985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -981,7 +995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -991,7 +1005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1001,7 +1015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -1011,7 +1025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -1021,7 +1035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>10</v>
       </c>
@@ -1065,9 +1079,9 @@
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>11</v>
       </c>
@@ -1076,14 +1090,14 @@
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
     </row>
-    <row r="2" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>12</v>
       </c>
@@ -1092,7 +1106,7 @@
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -1109,7 +1123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>41662</v>
       </c>
@@ -1127,7 +1141,7 @@
         <v>3.8194444444444031E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>41662</v>
       </c>
@@ -1145,7 +1159,7 @@
         <v>4.8611111111110938E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>41664</v>
       </c>
@@ -1163,7 +1177,7 @@
         <v>0.15972222222222199</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="17"/>
       <c r="C8" s="16"/>
@@ -1173,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="17"/>
       <c r="C9" s="16"/>
@@ -1183,7 +1197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="17"/>
       <c r="C10" s="16"/>
@@ -1193,7 +1207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="17"/>
       <c r="C11" s="16"/>
@@ -1203,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="17"/>
       <c r="C12" s="16"/>
@@ -1213,7 +1227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="17"/>
       <c r="C13" s="16"/>
@@ -1223,7 +1237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="16"/>
@@ -1233,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="17"/>
       <c r="C15" s="16"/>
@@ -1243,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="17"/>
       <c r="C16" s="16"/>
@@ -1253,7 +1267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="17"/>
       <c r="C17" s="16"/>
@@ -1263,7 +1277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="17"/>
       <c r="C18" s="16"/>
@@ -1273,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="17"/>
       <c r="C19" s="16"/>
@@ -1283,7 +1297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="17"/>
       <c r="C20" s="16"/>
@@ -1293,7 +1307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -1303,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -1313,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -1323,7 +1337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
@@ -1333,7 +1347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -1343,7 +1357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
@@ -1353,7 +1367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -1363,7 +1377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
@@ -1373,7 +1387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -1383,7 +1397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
@@ -1393,7 +1407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -1403,7 +1417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>10</v>
       </c>
@@ -1439,9 +1453,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
@@ -1450,14 +1464,14 @@
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>12</v>
       </c>
@@ -1466,7 +1480,7 @@
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -1483,77 +1497,77 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="17"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="17"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="17"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="17"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="17"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="17"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="17"/>
       <c r="C15" s="16"/>
@@ -1563,119 +1577,119 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="17"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="17"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="17"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="17"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="17"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="16"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="16"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
       <c r="E24" s="16"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
       <c r="E26" s="16"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
       <c r="E27" s="16"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
       <c r="E28" s="16"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="16"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="16"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
       <c r="E31" s="16"/>
     </row>
-    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>10</v>
       </c>
@@ -1707,13 +1721,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>17</v>
       </c>
@@ -1722,14 +1736,14 @@
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
     </row>
-    <row r="2" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>12</v>
       </c>
@@ -1738,7 +1752,7 @@
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -1755,196 +1769,204 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="E5" s="16"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="17"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="17"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="17"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="17"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="17"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="17"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="17"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="17"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="17"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="17"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="17"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="17"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="16"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="16"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
       <c r="E24" s="16"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
       <c r="E26" s="16"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
       <c r="E27" s="16"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
       <c r="E28" s="16"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="16"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="16"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
       <c r="E31" s="16"/>
     </row>
-    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>10</v>
       </c>
@@ -1980,9 +2002,9 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>18</v>
       </c>
@@ -1991,14 +2013,14 @@
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>12</v>
       </c>
@@ -2007,7 +2029,7 @@
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -2024,7 +2046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>41666</v>
       </c>
@@ -2042,7 +2064,7 @@
         <v>2.0833333333333037E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="16"/>
@@ -2052,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
@@ -2062,7 +2084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="17"/>
       <c r="C8" s="16"/>
@@ -2072,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="17"/>
       <c r="C9" s="16"/>
@@ -2082,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="17"/>
       <c r="C10" s="16"/>
@@ -2092,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="17"/>
       <c r="C11" s="16"/>
@@ -2102,7 +2124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="17"/>
       <c r="C12" s="16"/>
@@ -2112,7 +2134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="17"/>
       <c r="C13" s="16"/>
@@ -2122,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="16"/>
@@ -2132,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="17"/>
       <c r="C15" s="16"/>
@@ -2142,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="17"/>
       <c r="C16" s="16"/>
@@ -2152,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="17"/>
       <c r="C17" s="16"/>
@@ -2162,7 +2184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="17"/>
       <c r="C18" s="16"/>
@@ -2172,7 +2194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="17"/>
       <c r="C19" s="16"/>
@@ -2182,7 +2204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="17"/>
       <c r="C20" s="16"/>
@@ -2192,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -2202,7 +2224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
@@ -2212,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -2222,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
@@ -2232,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
@@ -2242,7 +2264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
@@ -2252,7 +2274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
@@ -2262,7 +2284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
@@ -2272,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -2282,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
@@ -2292,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -2302,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>10</v>
       </c>
@@ -2334,16 +2356,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="33.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>20</v>
       </c>
@@ -2352,14 +2374,14 @@
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
     </row>
-    <row r="2" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>12</v>
       </c>
@@ -2368,7 +2390,7 @@
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -2385,7 +2407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>41300</v>
       </c>
@@ -2402,7 +2424,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>41301</v>
       </c>
@@ -2419,182 +2441,182 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="17"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="17"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="17"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="17"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="17"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="17"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="17"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="17"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="17"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="17"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="17"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="17"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="20"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
       <c r="E31" s="21"/>
     </row>
-    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>10</v>
       </c>

</xml_diff>